<commit_message>
Some Minor Alterations before the pull
</commit_message>
<xml_diff>
--- a/CalendarData.xlsx
+++ b/CalendarData.xlsx
@@ -1,55 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:loext="http://schemas.libreoffice.org/" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fileVersion appName="Calc"/>
-  <x:workbookPr date1904="false" showObjects="all" backupFile="false" codeName="ThisWorkbook"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:workbookPr codeName="ThisWorkbook"/>
   <x:bookViews>
-    <x:workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr refMode="A1" iterate="false" iterateCount="100" iterateDelta="0.0001"/>
-  <x:extLst>
-    <x:ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </x:ext>
-  </x:extLst>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <x:si>
     <x:t>20</x:t>
   </x:si>
   <x:si>
-    <x:t>12:15 – 12:45pm</x:t>
+    <x:t>12 – 1pm</x:t>
   </x:si>
   <x:si>
     <x:t>MAY</x:t>
   </x:si>
   <x:si>
-    <x:t>Event D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 – 4:30pm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Event E</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 – 4:30am</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Event F</x:t>
+    <x:t>Event A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Event FL</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -57,31 +39,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
-    <x:numFmt numFmtId="164" formatCode="General"/>
+    <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="5">
-    <x:font>
-      <x:sz val="10"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Arial"/>
-      <x:family val="0"/>
-      <x:charset val="1"/>
-    </x:font>
-    <x:font>
-      <x:sz val="10"/>
-      <x:name val="Arial"/>
-      <x:family val="0"/>
-    </x:font>
-    <x:font>
-      <x:sz val="10"/>
-      <x:name val="Arial"/>
-      <x:family val="0"/>
-    </x:font>
-    <x:font>
-      <x:sz val="10"/>
-      <x:name val="Arial"/>
-      <x:family val="0"/>
-    </x:font>
+  <x:fonts count="1">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -99,70 +59,37 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="false" diagonalDown="false">
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="22">
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <x:protection locked="true" hidden="false"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <x:xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <x:protection locked="true" hidden="false"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <x:protection locked="true" hidden="false"/>
-    </x:xf>
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="6">
+  <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <x:cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <x:cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <x:cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <x:cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <x:cellStyle name="Percent" xfId="19" builtinId="5"/>
   </x:cellStyles>
 </x:styleSheet>
 </file>
@@ -450,78 +377,50 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr filterMode="false">
+  <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
-    <x:pageSetUpPr fitToPage="false"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:D2"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" defaultGridColor="true" topLeftCell="A1" colorId="64" workbookViewId="0">
-      <x:selection activeCell="H15" sqref="H15 H15:H15"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="12.8" zeroHeight="false"/>
-  <x:cols>
-    <x:col min="1" max="1" width="35.29" style="3" customWidth="1"/>
-    <x:col min="2" max="1025" width="15.15" style="3" customWidth="1"/>
-  </x:cols>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1025" customFormat="1" ht="23.1" customHeight="1" outlineLevel="0">
-      <x:c r="A1" s="2" t="s">
+    <x:row r="1" spans="1:4">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
+      <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1025" customFormat="1" ht="18.65" customHeight="1" outlineLevel="0">
-      <x:c r="A2" s="2" t="s">
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="s">
+      <x:c r="B2" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D2" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
     </x:row>
-    <x:row r="3" spans="1:1025">
-      <x:c r="A3" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B3" s="3" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C3" s="3" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D3" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:1025">
-      <x:c r="H15" s="3" t="s"/>
-    </x:row>
-    <x:row r="1048576" spans="1:1025" customFormat="1" ht="12.8" customHeight="1" outlineLevel="0"/>
   </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="true"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.511805555555555" footer="0.511805555555555"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <x:headerFooter differentOddEven="false" differentFirst="false">
-    <x:oddHeader/>
-    <x:oddFooter/>
-  </x:headerFooter>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed already existing credentials password error for real this time.
</commit_message>
<xml_diff>
--- a/CalendarData.xlsx
+++ b/CalendarData.xlsx
@@ -14,24 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <x:si>
     <x:t>20</x:t>
   </x:si>
   <x:si>
-    <x:t>12 – 1pm</x:t>
+    <x:t>12:15 – 12:45pm</x:t>
   </x:si>
   <x:si>
     <x:t>MAY</x:t>
   </x:si>
   <x:si>
-    <x:t>Event A</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Event FL</x:t>
+    <x:t>Event D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 – 4:30pm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Event E</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 – 4:30am</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Event F</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -407,13 +419,27 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Deleting the useless main
</commit_message>
<xml_diff>
--- a/CalendarData.xlsx
+++ b/CalendarData.xlsx
@@ -14,36 +14,192 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+  <x:si>
+    <x:t>31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>All day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MAY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Memorial Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JUN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Juneteenth</x:t>
+  </x:si>
   <x:si>
     <x:t>20</x:t>
   </x:si>
   <x:si>
-    <x:t>12:15 – 12:45pm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MAY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Event D</x:t>
+    <x:t>Father's Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JUL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Independence Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Independence Day observed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Labor Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>First Day of Hispanic Heritage Month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Columbus Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Halloween</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NOV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Election Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daylight Saving Time ends</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Veterans Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thanksgiving Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Native American Heritage Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DEC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Christmas Eve</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Christmas Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Day off for New Year's Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New Year's Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Martin Luther King Jr. Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FEB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>First Day of Black History Month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valentine's Day</x:t>
   </x:si>
   <x:si>
     <x:t>21</x:t>
   </x:si>
   <x:si>
-    <x:t>4 – 4:30pm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Event E</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4 – 4:30am</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Event F</x:t>
+    <x:t>Presidents' Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MAR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>First Day of Women's History Month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Daylight Saving Time starts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>St. Patrick's Day</x:t>
+  </x:si>
+  <x:si>
+    <x:t>APR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Easter Sunday</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Easter Monday</x:t>
+  </x:si>
+  <x:si>
+    <x:t>First Day of Asian American and Pacific Islander Heritage Month</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cinco de Mayo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mother's Day</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -419,10 +575,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>5</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>2</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>6</x:v>
@@ -433,13 +589,391 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:4">
+      <x:c r="A6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:4">
+      <x:c r="A7" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:4">
+      <x:c r="A8" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:4">
+      <x:c r="A9" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:4">
+      <x:c r="A10" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:4">
+      <x:c r="A11" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="A12" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="A13" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="A14" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="A15" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="A16" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="A17" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="A18" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="A19" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="A20" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="A21" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="A22" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="A23" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="A24" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="A25" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="A26" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>9</x:v>
+      <x:c r="D28" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>